<commit_message>
flexible start date for the reservoir storage
modifying the flexible start date feature for the reservoir storage
</commit_message>
<xml_diff>
--- a/gui_key.xlsx
+++ b/gui_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/danli_ad_unc_edu/Documents/github/CALFEWS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/danli_ad_unc_edu/Documents/github/CALFEWS_waterFutures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{E833FA7A-AF5B-4B59-A5BF-C99FA643A5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28B0C9F6-03FC-406A-A6C7-0E99A0DFC174}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{E833FA7A-AF5B-4B59-A5BF-C99FA643A5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{882EF85C-EA3F-4D23-B876-AD90BC00BCF8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="727" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="727" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_data" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="589">
   <si>
     <t>Object List</t>
   </si>
@@ -204,9 +204,6 @@
     <t>TRP_pump</t>
   </si>
   <si>
-    <t>Pumping through Jones pumping plant (CVP)</t>
-  </si>
-  <si>
     <t>km</t>
   </si>
   <si>
@@ -1806,7 +1803,7 @@
     <t>CDEC_1995_2023</t>
   </si>
   <si>
-    <t>DNP_precip</t>
+    <t xml:space="preserve">Pumping through Jones/Tracy pumping plant (CVP) </t>
   </si>
 </sst>
 </file>
@@ -2257,599 +2254,599 @@
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>570</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>571</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>321</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>585</v>
+      </c>
+      <c r="B2" t="s">
         <v>586</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F2" t="s">
         <v>587</v>
-      </c>
-      <c r="D2" t="s">
-        <v>323</v>
-      </c>
-      <c r="E2" t="s">
-        <v>324</v>
-      </c>
-      <c r="F2" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C3">
         <v>11</v>
       </c>
       <c r="D3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E3" t="s">
         <v>323</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>324</v>
-      </c>
-      <c r="F3" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C4">
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E4" t="s">
+        <v>323</v>
+      </c>
+      <c r="F4" t="s">
         <v>324</v>
-      </c>
-      <c r="F4" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C6">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E6" t="s">
+        <v>331</v>
+      </c>
+      <c r="F6" t="s">
         <v>332</v>
-      </c>
-      <c r="F6" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B7" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B8" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E8" t="s">
+        <v>329</v>
+      </c>
+      <c r="F8" t="s">
         <v>330</v>
-      </c>
-      <c r="F8" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>524</v>
+      </c>
+      <c r="B9" t="s">
         <v>525</v>
-      </c>
-      <c r="B9" t="s">
-        <v>526</v>
       </c>
       <c r="C9">
         <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E9" t="s">
+        <v>526</v>
+      </c>
+      <c r="F9" t="s">
         <v>527</v>
-      </c>
-      <c r="F9" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B10" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C10">
         <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E10" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F10" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B11" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C11">
         <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E11" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F11" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B12" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C12">
         <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E12" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F12" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C13">
         <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E13" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B14" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C14">
         <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E14" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F14" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B15" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C15">
         <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E15" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F15" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B16" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C16">
         <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E16" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F16" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B17" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C17">
         <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E17" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F17" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B18" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C18">
         <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E18" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F18" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B19" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C19">
         <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E19" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F19" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B20" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C20">
         <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E20" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F20" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B21" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C21">
         <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E21" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F21" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B22" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C22">
         <v>76</v>
       </c>
       <c r="D22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E22" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F22" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B23" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C23">
         <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E23" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F23" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B24" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C24">
         <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E24" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F24" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B25" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C25">
         <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E25" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F25" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B26" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C26">
         <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E26" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B27" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C27">
         <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E27" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F27" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B28" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C28">
         <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E28" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F28" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B29" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C29">
         <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E29" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F29" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B30" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C30">
         <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E30" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F30" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
   </sheetData>
@@ -2883,51 +2880,51 @@
         <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" t="s">
         <v>176</v>
-      </c>
-      <c r="B2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" t="s">
         <v>178</v>
-      </c>
-      <c r="B3" t="s">
-        <v>262</v>
-      </c>
-      <c r="C3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" t="s">
         <v>174</v>
-      </c>
-      <c r="B4" t="s">
-        <v>261</v>
-      </c>
-      <c r="C4" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C5" t="s">
         <v>172</v>
-      </c>
-      <c r="B5" t="s">
-        <v>260</v>
-      </c>
-      <c r="C5" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -2966,13 +2963,13 @@
         <v>4</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
@@ -2980,10 +2977,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -2992,15 +2989,15 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -3009,15 +3006,15 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -3026,15 +3023,15 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -3043,15 +3040,15 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -3060,15 +3057,15 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -3077,15 +3074,15 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -3094,15 +3091,15 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -3111,15 +3108,15 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B10" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -3128,15 +3125,15 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B11" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -3145,15 +3142,15 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B12" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -3162,15 +3159,15 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -3179,15 +3176,15 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -3196,15 +3193,15 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B15" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -3213,15 +3210,15 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -3230,15 +3227,15 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B17" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -3247,15 +3244,15 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B18" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -3264,15 +3261,15 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -3281,15 +3278,15 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B20" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -3298,15 +3295,15 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B21" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -3315,15 +3312,15 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B22" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -3332,7 +3329,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -3364,150 +3361,150 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2" t="s">
         <v>468</v>
       </c>
-      <c r="B2" t="s">
-        <v>469</v>
-      </c>
       <c r="C2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>464</v>
+      </c>
+      <c r="B5" t="s">
         <v>465</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>466</v>
-      </c>
-      <c r="C5" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>461</v>
+      </c>
+      <c r="B6" t="s">
         <v>462</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>463</v>
-      </c>
-      <c r="C6" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B8" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>455</v>
+      </c>
+      <c r="B10" t="s">
         <v>456</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>457</v>
-      </c>
-      <c r="C10" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>458</v>
+      </c>
+      <c r="B11" t="s">
         <v>459</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>460</v>
-      </c>
-      <c r="C11" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B12" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>579</v>
+      </c>
+      <c r="B13" t="s">
         <v>580</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>581</v>
-      </c>
-      <c r="C13" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>582</v>
+      </c>
+      <c r="B14" t="s">
         <v>583</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>584</v>
-      </c>
-      <c r="C14" t="s">
-        <v>585</v>
       </c>
     </row>
   </sheetData>
@@ -3542,13 +3539,13 @@
         <v>4</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
@@ -3556,10 +3553,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -3568,7 +3565,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -3602,7 +3599,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -3613,7 +3610,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -3624,7 +3621,7 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -3635,7 +3632,7 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -3646,7 +3643,7 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -3657,7 +3654,7 @@
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -3668,7 +3665,7 @@
         <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -3679,7 +3676,7 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -3690,7 +3687,7 @@
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -3701,7 +3698,7 @@
         <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -3712,7 +3709,7 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -3723,7 +3720,7 @@
         <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -3734,7 +3731,7 @@
         <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -3745,7 +3742,7 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -3756,7 +3753,7 @@
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3788,13 +3785,13 @@
         <v>4</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
@@ -3805,7 +3802,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -3822,7 +3819,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -3839,7 +3836,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -3848,7 +3845,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -3856,7 +3853,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -3865,15 +3862,15 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -3882,32 +3879,32 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C7" t="s">
         <v>279</v>
       </c>
-      <c r="B7" t="s">
-        <v>355</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>280</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -3916,15 +3913,15 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -3933,7 +3930,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -3941,7 +3938,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -3958,7 +3955,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -3975,7 +3972,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -3992,7 +3989,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
@@ -4006,10 +4003,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>366</v>
+      </c>
+      <c r="B14" t="s">
         <v>367</v>
-      </c>
-      <c r="B14" t="s">
-        <v>368</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -4018,15 +4015,15 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="B15" t="s">
         <v>369</v>
-      </c>
-      <c r="B15" t="s">
-        <v>370</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -4035,7 +4032,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -4067,7 +4064,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -4078,7 +4075,7 @@
         <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -4096,7 +4093,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4113,13 +4110,13 @@
         <v>4</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
@@ -4127,10 +4124,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -4139,15 +4136,15 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -4156,15 +4153,15 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -4173,7 +4170,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -4181,7 +4178,7 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -4190,7 +4187,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>588</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -4198,7 +4195,7 @@
         <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -4212,10 +4209,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -4224,15 +4221,15 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -4241,15 +4238,15 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -4258,15 +4255,15 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -4275,16 +4272,16 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -4293,15 +4290,15 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B12" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -4310,15 +4307,15 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B13" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -4327,15 +4324,15 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B14" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -4344,58 +4341,58 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>372</v>
+      </c>
+      <c r="C15" t="s">
         <v>62</v>
       </c>
-      <c r="B15" t="s">
-        <v>373</v>
-      </c>
-      <c r="C15" t="s">
-        <v>63</v>
-      </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -4412,7 +4409,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P8" sqref="P8:P9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4427,153 +4424,153 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D2" t="s">
         <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>433</v>
-      </c>
-      <c r="C2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D3" t="s">
         <v>76</v>
-      </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C4" t="s">
         <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D5" t="s">
         <v>80</v>
-      </c>
-      <c r="B5" t="s">
-        <v>434</v>
-      </c>
-      <c r="C5" t="s">
-        <v>288</v>
-      </c>
-      <c r="D5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>436</v>
+      </c>
+      <c r="C8" t="s">
+        <v>393</v>
+      </c>
+      <c r="D8" t="s">
         <v>88</v>
-      </c>
-      <c r="B8" t="s">
-        <v>437</v>
-      </c>
-      <c r="C8" t="s">
-        <v>394</v>
-      </c>
-      <c r="D8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
         <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>437</v>
+      </c>
+      <c r="C10" t="s">
+        <v>289</v>
+      </c>
+      <c r="D10" t="s">
         <v>84</v>
-      </c>
-      <c r="B10" t="s">
-        <v>438</v>
-      </c>
-      <c r="C10" t="s">
-        <v>290</v>
-      </c>
-      <c r="D10" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="s">
+        <v>438</v>
+      </c>
+      <c r="C11" t="s">
+        <v>288</v>
+      </c>
+      <c r="D11" t="s">
         <v>82</v>
-      </c>
-      <c r="B11" t="s">
-        <v>439</v>
-      </c>
-      <c r="C11" t="s">
-        <v>289</v>
-      </c>
-      <c r="D11" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -4591,7 +4588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4609,13 +4606,13 @@
         <v>4</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>6</v>
@@ -4623,10 +4620,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -4635,15 +4632,15 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -4652,15 +4649,15 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -4669,15 +4666,15 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -4686,15 +4683,15 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -4703,15 +4700,15 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -4720,15 +4717,15 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -4737,7 +4734,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -4747,10 +4744,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4763,7 +4760,7 @@
     <col min="6" max="6" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -4771,626 +4768,623 @@
         <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C7" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" t="s">
+        <v>453</v>
+      </c>
+      <c r="C9" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" t="s">
+        <v>454</v>
+      </c>
+      <c r="C12" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C13" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>119</v>
       </c>
-      <c r="B3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C3" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" t="s">
-        <v>206</v>
-      </c>
-      <c r="C4" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C5" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C6" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" t="s">
-        <v>208</v>
-      </c>
-      <c r="C7" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C14" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" t="s">
         <v>238</v>
       </c>
-      <c r="C8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B9" t="s">
-        <v>454</v>
-      </c>
-      <c r="C9" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" t="s">
-        <v>235</v>
-      </c>
-      <c r="C11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B12" t="s">
-        <v>455</v>
-      </c>
-      <c r="C12" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>171</v>
-      </c>
-      <c r="B13" t="s">
-        <v>254</v>
-      </c>
-      <c r="C13" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" t="s">
-        <v>221</v>
-      </c>
-      <c r="C14" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" t="s">
-        <v>239</v>
-      </c>
       <c r="C15" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C16" t="s">
-        <v>409</v>
-      </c>
-      <c r="F16" t="s">
-        <v>589</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C18" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" t="s">
         <v>101</v>
-      </c>
-      <c r="B19" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" t="s">
         <v>114</v>
-      </c>
-      <c r="B21" t="s">
-        <v>218</v>
-      </c>
-      <c r="C21" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C22" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C23" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" t="s">
+        <v>249</v>
+      </c>
+      <c r="C24" t="s">
         <v>165</v>
-      </c>
-      <c r="B24" t="s">
-        <v>250</v>
-      </c>
-      <c r="C24" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C25" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C26" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C27" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C28" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B29" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C29" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C30" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C31" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C32" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C33" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C34" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" t="s">
+        <v>251</v>
+      </c>
+      <c r="C35" t="s">
         <v>168</v>
-      </c>
-      <c r="B35" t="s">
-        <v>252</v>
-      </c>
-      <c r="C35" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C36" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C37" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B38" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C38" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" t="s">
+        <v>236</v>
+      </c>
+      <c r="C39" t="s">
         <v>139</v>
-      </c>
-      <c r="B39" t="s">
-        <v>237</v>
-      </c>
-      <c r="C39" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" t="s">
+        <v>235</v>
+      </c>
+      <c r="C40" t="s">
         <v>137</v>
-      </c>
-      <c r="B40" t="s">
-        <v>236</v>
-      </c>
-      <c r="C40" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C41" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B42" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C42" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C43" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C44" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C46" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B47" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C47" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C48" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" t="s">
+        <v>239</v>
+      </c>
+      <c r="C49" t="s">
         <v>145</v>
-      </c>
-      <c r="B49" t="s">
-        <v>240</v>
-      </c>
-      <c r="C49" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B50" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C50" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B51" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B52" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53" t="s">
+        <v>245</v>
+      </c>
+      <c r="C53" t="s">
         <v>157</v>
-      </c>
-      <c r="B53" t="s">
-        <v>246</v>
-      </c>
-      <c r="C53" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B54" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C54" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B55" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C55" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>159</v>
+      </c>
+      <c r="B56" t="s">
+        <v>247</v>
+      </c>
+      <c r="C56" t="s">
         <v>160</v>
-      </c>
-      <c r="B56" t="s">
-        <v>248</v>
-      </c>
-      <c r="C56" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C57" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -5406,7 +5400,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5426,13 +5420,13 @@
         <v>4</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>6</v>
@@ -5440,10 +5434,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -5452,15 +5446,15 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -5469,15 +5463,15 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -5486,15 +5480,15 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -5503,15 +5497,15 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -5520,15 +5514,15 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -5537,15 +5531,15 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B8" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -5554,15 +5548,15 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -5571,15 +5565,15 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B10" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -5588,15 +5582,15 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B11" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -5605,15 +5599,15 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -5622,15 +5616,15 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -5639,15 +5633,15 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -5656,15 +5650,15 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -5673,15 +5667,15 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -5690,15 +5684,15 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -5707,15 +5701,15 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -5724,15 +5718,15 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -5741,15 +5735,15 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B20" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -5758,15 +5752,15 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B21" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -5775,15 +5769,15 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B22" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -5792,7 +5786,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update input file (with correct water year)
</commit_message>
<xml_diff>
--- a/gui_key.xlsx
+++ b/gui_key.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{E833FA7A-AF5B-4B59-A5BF-C99FA643A5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{882EF85C-EA3F-4D23-B876-AD90BC00BCF8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="727" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27120" yWindow="3780" windowWidth="17784" windowHeight="11712" tabRatio="727" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_data" sheetId="7" r:id="rId1"/>
@@ -4092,8 +4092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4746,7 +4746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
recent update on post-processing index-insurance strategy
</commit_message>
<xml_diff>
--- a/gui_key.xlsx
+++ b/gui_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/danli_ad_unc_edu/Documents/github/CALFEWS_waterFutures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{E833FA7A-AF5B-4B59-A5BF-C99FA643A5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{882EF85C-EA3F-4D23-B876-AD90BC00BCF8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABA9E07-7A52-4439-B1A2-0C6EEF77A11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27120" yWindow="3780" windowWidth="17784" windowHeight="11712" tabRatio="727" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="783" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_data" sheetId="7" r:id="rId1"/>
@@ -1968,10 +1968,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3578,9 +3574,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H13" sqref="H13"/>
+      <selection pane="topRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4092,13 +4088,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.81640625" customWidth="1"/>
     <col min="3" max="3" width="12.81640625" customWidth="1"/>
     <col min="4" max="4" width="6.90625" bestFit="1" customWidth="1"/>

</xml_diff>